<commit_message>
Improve the legacy data migration by adding support for appliance types
Implements appliance type mapping in ExcelService and LegacyDataImporter, updates legacy data import script, and adds documentation in legacy-migration-guide.md.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 866a9aad-2ef4-41b0-a844-34662a56feff
</commit_message>
<xml_diff>
--- a/test-klijenti-za-uvoz.xlsx
+++ b/test-klijenti-za-uvoz.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -504,9 +504,26 @@
         <v/>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Marko Petrović</v>
+      </c>
+      <c r="B7" t="str">
+        <v>069/987-654</v>
+      </c>
+      <c r="C7" t="str">
+        <v>Kotor</v>
+      </c>
+      <c r="D7" t="str">
+        <v/>
+      </c>
+      <c r="E7" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add support for combined refrigerators during legacy data import
Extends appliance type mapping to include "Kombinovan frižider" variations in ExcelService and legacy data import scripts.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 866a9aad-2ef4-41b0-a844-34662a56feff
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/883c0e1c-965e-403d-8bc0-39adca99d551/866a9aad-2ef4-41b0-a844-34662a56feff/ZmQ3RE7
</commit_message>
<xml_diff>
--- a/test-klijenti-za-uvoz.xlsx
+++ b/test-klijenti-za-uvoz.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -521,9 +521,26 @@
         <v/>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Ana Milic</v>
+      </c>
+      <c r="B8" t="str">
+        <v>067/777-888</v>
+      </c>
+      <c r="C8" t="str">
+        <v>Tivat</v>
+      </c>
+      <c r="D8" t="str">
+        <v/>
+      </c>
+      <c r="E8" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E7"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>